<commit_message>
Upload com as tabelas finais de internações por morbidade em CID 10. Ativação dos filtros necessários para realizar a pesquisa corretamente.
</commit_message>
<xml_diff>
--- a/doc/pesquisas-estudos/Estudos/Internações/Internacoes por morbidade em CID_10.xlsx
+++ b/doc/pesquisas-estudos/Estudos/Internações/Internacoes por morbidade em CID_10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucen\FATEC\API COVID_LONGA\Cloned_Projekt\API_1\doc\pesquisas-estudos\Estudos\Internações\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDC4A2B-3147-42E9-927F-DA4691D3311B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A35676C-0D6B-4764-8C76-F4A64A4C75E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" firstSheet="6" activeTab="8" xr2:uid="{8010108B-CAA3-491B-95F9-021E8440CA4D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="3" activeTab="3" xr2:uid="{8010108B-CAA3-491B-95F9-021E8440CA4D}"/>
   </bookViews>
   <sheets>
     <sheet name="CID I" sheetId="1" r:id="rId1"/>
@@ -1097,7 +1097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED31A10-BCB0-4A4D-9B45-F6708FB5032E}">
   <dimension ref="A1:U54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection sqref="A1:A16"/>
     </sheetView>
   </sheetViews>
@@ -3755,13 +3755,13 @@
     <mergeCell ref="J38:J39"/>
     <mergeCell ref="K38:K39"/>
     <mergeCell ref="L38:L39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
     <mergeCell ref="R20:R21"/>
     <mergeCell ref="S20:S21"/>
     <mergeCell ref="T20:T21"/>
     <mergeCell ref="P19:P21"/>
     <mergeCell ref="Q19:T19"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
     <mergeCell ref="M20:M21"/>
     <mergeCell ref="N20:N34"/>
     <mergeCell ref="Q20:Q21"/>
@@ -5409,15 +5409,15 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="P1:P3"/>
     <mergeCell ref="N2:N16"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
     <mergeCell ref="A19:A34"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="I19:I21"/>
     <mergeCell ref="J19:M19"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
     <mergeCell ref="U2:U16"/>
     <mergeCell ref="T20:T21"/>
     <mergeCell ref="P19:P21"/>
@@ -5467,8 +5467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39DA4F03-68DF-4C6B-8B1C-8B8A9D284961}">
   <dimension ref="A1:U54"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8087,8 +8087,6 @@
     <mergeCell ref="T38:T39"/>
     <mergeCell ref="E38:E39"/>
     <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G52"/>
-    <mergeCell ref="J38:J39"/>
     <mergeCell ref="R20:R21"/>
     <mergeCell ref="M38:M39"/>
     <mergeCell ref="N38:N52"/>
@@ -8105,6 +8103,8 @@
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="K38:K39"/>
     <mergeCell ref="L38:L39"/>
+    <mergeCell ref="G38:G52"/>
+    <mergeCell ref="J38:J39"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="M2:M3"/>
@@ -8146,8 +8146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CDB44BD-9456-434D-919F-CA804237705E}">
   <dimension ref="A1:U54"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:A34"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56:H108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10650,8 +10650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1411F88C-9079-439D-8B5F-77073FA8E111}">
   <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView tabSelected="1" topLeftCell="C84" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55:Q107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13013,7 +13013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88A4C35-C715-46F7-B815-82F5F4D5BF44}">
   <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
@@ -17112,8 +17112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A533D09A-58F2-42A5-AF0A-EC46D65715B8}">
   <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="P55" sqref="P55"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19492,22 +19492,20 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="Q1:T1"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G16"/>
-    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="P1:P3"/>
+    <mergeCell ref="N2:N16"/>
+    <mergeCell ref="S2:S3"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:M1"/>
-    <mergeCell ref="P1:P3"/>
-    <mergeCell ref="N2:N16"/>
-    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G16"/>
+    <mergeCell ref="J2:J3"/>
     <mergeCell ref="T2:T3"/>
     <mergeCell ref="U2:U16"/>
     <mergeCell ref="A19:A34"/>
@@ -19522,6 +19520,8 @@
     <mergeCell ref="L20:L21"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="R2:R3"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="C2:C3"/>
     <mergeCell ref="Q37:T37"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="D38:D39"/>
@@ -19566,10 +19566,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA0FF6EE-4FA5-4C0A-BC96-3B41A8EB8A71}">
-  <dimension ref="A1:U52"/>
+  <dimension ref="A1:U81"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="R54" sqref="R54"/>
+    <sheetView topLeftCell="H10" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55:I107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22040,6 +22040,54 @@
       </c>
       <c r="U52" s="77"/>
     </row>
+    <row r="70" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J70" s="30"/>
+      <c r="K70" s="30"/>
+    </row>
+    <row r="71" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J71" s="30"/>
+      <c r="K71" s="30"/>
+    </row>
+    <row r="72" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J72" s="30"/>
+      <c r="K72" s="30"/>
+    </row>
+    <row r="73" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J73" s="30"/>
+      <c r="K73" s="30"/>
+    </row>
+    <row r="74" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J74" s="30"/>
+      <c r="K74" s="30"/>
+    </row>
+    <row r="75" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J75" s="30"/>
+      <c r="K75" s="30"/>
+    </row>
+    <row r="76" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J76" s="30"/>
+      <c r="K76" s="30"/>
+    </row>
+    <row r="77" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J77" s="30"/>
+      <c r="K77" s="30"/>
+    </row>
+    <row r="78" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J78" s="30"/>
+      <c r="K78" s="30"/>
+    </row>
+    <row r="79" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J79" s="30"/>
+      <c r="K79" s="30"/>
+    </row>
+    <row r="80" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J80" s="30"/>
+      <c r="K80" s="30"/>
+    </row>
+    <row r="81" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J81" s="30"/>
+      <c r="K81" s="30"/>
+    </row>
   </sheetData>
   <mergeCells count="66">
     <mergeCell ref="A1:A16"/>
@@ -22059,15 +22107,15 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="P1:P3"/>
     <mergeCell ref="N2:N16"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
     <mergeCell ref="A19:A34"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="I19:I21"/>
     <mergeCell ref="J19:M19"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
     <mergeCell ref="U2:U16"/>
     <mergeCell ref="T20:T21"/>
     <mergeCell ref="P19:P21"/>
@@ -22117,7 +22165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C05C3D1A-E010-4FE6-A647-8C2054374453}">
   <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
@@ -24318,15 +24366,15 @@
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="P1:P3"/>
     <mergeCell ref="N2:N16"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
     <mergeCell ref="A19:A34"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="I19:I21"/>
     <mergeCell ref="J19:M19"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
     <mergeCell ref="U2:U16"/>
     <mergeCell ref="T20:T21"/>
     <mergeCell ref="P19:P21"/>

</xml_diff>